<commit_message>
All data loaded in mlruns
</commit_message>
<xml_diff>
--- a/Data/UN Population Data/Sweden.xlsx
+++ b/Data/UN Population Data/Sweden.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sean\Documents\Modelling\Data\UN Population Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\modelling\Data\UN Population Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="65">
   <si>
     <t>…</t>
   </si>
@@ -214,12 +214,18 @@
   </si>
   <si>
     <t>20 +</t>
+  </si>
+  <si>
+    <t>14-under</t>
+  </si>
+  <si>
+    <t>15+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#\ ###\ ###\ ##0;\-#\ ###\ ###\ ##0;0"/>
     <numFmt numFmtId="165" formatCode="##0.0;\-##0.0;0"/>
@@ -531,10 +537,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -546,25 +570,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -849,10 +855,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:X29"/>
+  <dimension ref="B1:X35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2237,6 +2243,24 @@
       <c r="M29" s="11"/>
       <c r="N29" s="11"/>
     </row>
+    <row r="34" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>63</v>
+      </c>
+      <c r="H34" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G35" s="8">
+        <f>SUM(C17:E17)*1000</f>
+        <v>1688811.0000000002</v>
+      </c>
+      <c r="H35" s="8">
+        <f>SUM(F17:X17)*1000</f>
+        <v>8074754.0000000009</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="E24:F24"/>
@@ -2252,7 +2276,7 @@
   <dimension ref="B2:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2267,16 +2291,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
       <c r="J2" s="13"/>
     </row>
     <row r="3" spans="2:16" ht="45" x14ac:dyDescent="0.25">
@@ -2309,7 +2333,7 @@
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B4" s="38">
+      <c r="B4" s="34">
         <v>1</v>
       </c>
       <c r="C4" s="20" t="s">
@@ -2326,25 +2350,25 @@
         <f>E4/SUM($E$4:$E$6)</f>
         <v>0.27334601900459482</v>
       </c>
-      <c r="G4" s="32">
+      <c r="G4" s="33">
         <f>SUM(D4*F4,D5*F5,D6*F6)</f>
         <v>3.9768679942169527</v>
       </c>
-      <c r="H4" s="32">
+      <c r="H4" s="33">
         <f>SUM(E4:E6)*1000</f>
         <v>2174632</v>
       </c>
-      <c r="I4" s="32">
+      <c r="I4" s="33">
         <f>H4*(G4/100)</f>
         <v>86482.243999999992</v>
       </c>
-      <c r="J4" s="31">
+      <c r="J4" s="38">
         <f>H4-I4</f>
         <v>2088149.7560000001</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B5" s="38"/>
+      <c r="B5" s="34"/>
       <c r="C5" s="24" t="s">
         <v>4</v>
       </c>
@@ -2359,15 +2383,15 @@
         <f>E5/SUM($E$4:$E$6)</f>
         <v>0.26204387684904851</v>
       </c>
-      <c r="G5" s="32"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="32"/>
-      <c r="J5" s="31"/>
+      <c r="G5" s="33"/>
+      <c r="H5" s="33"/>
+      <c r="I5" s="33"/>
+      <c r="J5" s="38"/>
       <c r="O5" s="26"/>
       <c r="P5" s="26"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="38"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="24" t="s">
         <v>29</v>
       </c>
@@ -2382,15 +2406,15 @@
         <f>E6/SUM($E$4:$E$6)</f>
         <v>0.46461010414635673</v>
       </c>
-      <c r="G6" s="32"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="32"/>
-      <c r="J6" s="31"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="38"/>
       <c r="O6" s="9"/>
       <c r="P6" s="9"/>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="38">
+      <c r="B7" s="34">
         <v>2</v>
       </c>
       <c r="C7" s="23" t="s">
@@ -2407,26 +2431,26 @@
         <f>E7/SUM($E$7:$E$8)</f>
         <v>0.36357401346305229</v>
       </c>
-      <c r="G7" s="32">
+      <c r="G7" s="33">
         <f>SUM(D7*F7,D8*F8)</f>
         <v>2.4632996727004821</v>
       </c>
-      <c r="H7" s="32">
+      <c r="H7" s="33">
         <f>SUM(E7:E8)*1000</f>
         <v>6661788</v>
       </c>
-      <c r="I7" s="32">
+      <c r="I7" s="33">
         <f>H7*(G7/100)</f>
         <v>164099.802</v>
       </c>
-      <c r="J7" s="33">
+      <c r="J7" s="39">
         <f>H7-I7</f>
         <v>6497688.1979999999</v>
       </c>
       <c r="O7" s="8"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="39"/>
+      <c r="B8" s="35"/>
       <c r="C8" s="9" t="s">
         <v>31</v>
       </c>
@@ -2444,19 +2468,19 @@
       <c r="G8" s="30"/>
       <c r="H8" s="30"/>
       <c r="I8" s="30"/>
-      <c r="J8" s="34"/>
+      <c r="J8" s="40"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
       <c r="J11" s="13"/>
     </row>
     <row r="12" spans="2:16" ht="45" x14ac:dyDescent="0.25">
@@ -2489,7 +2513,7 @@
       </c>
     </row>
     <row r="13" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="38">
+      <c r="B13" s="34">
         <v>1</v>
       </c>
       <c r="C13" s="20" t="s">
@@ -2506,25 +2530,25 @@
         <f>E13/SUM($E$13:$E$15)</f>
         <v>0.26767998979233781</v>
       </c>
-      <c r="G13" s="32">
+      <c r="G13" s="33">
         <f>SUM(D13*F13,D14*F14,D15*F15)</f>
         <v>4.0012499829112791</v>
       </c>
-      <c r="H13" s="32">
+      <c r="H13" s="33">
         <f>SUM(E13:E15)*1000</f>
         <v>2194430.0000000005</v>
       </c>
-      <c r="I13" s="32">
+      <c r="I13" s="33">
         <f>H13*(G13/100)</f>
         <v>87804.63</v>
       </c>
-      <c r="J13" s="31">
+      <c r="J13" s="38">
         <f>H13-I13</f>
         <v>2106625.3700000006</v>
       </c>
     </row>
     <row r="14" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="38"/>
+      <c r="B14" s="34"/>
       <c r="C14" s="24" t="s">
         <v>4</v>
       </c>
@@ -2539,13 +2563,13 @@
         <f t="shared" ref="F14:F15" si="0">E14/SUM($E$13:$E$15)</f>
         <v>0.26515085922084547</v>
       </c>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="31"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
+      <c r="J14" s="38"/>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="38"/>
+      <c r="B15" s="34"/>
       <c r="C15" s="24" t="s">
         <v>29</v>
       </c>
@@ -2560,13 +2584,13 @@
         <f t="shared" si="0"/>
         <v>0.46716915098681661</v>
       </c>
-      <c r="G15" s="32"/>
-      <c r="H15" s="32"/>
-      <c r="I15" s="32"/>
-      <c r="J15" s="31"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+      <c r="J15" s="38"/>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="38">
+      <c r="B16" s="34">
         <v>2</v>
       </c>
       <c r="C16" s="23" t="s">
@@ -2583,25 +2607,25 @@
         <f>E16/SUM($E$16:$E$17)</f>
         <v>0.34012340908175098</v>
       </c>
-      <c r="G16" s="32">
+      <c r="G16" s="33">
         <f>SUM(D16*F16,D17*F17)</f>
         <v>2.3366664090414555</v>
       </c>
-      <c r="H16" s="32">
+      <c r="H16" s="33">
         <f>SUM(E16:E17)*1000</f>
         <v>7569135.0000000019</v>
       </c>
-      <c r="I16" s="41">
+      <c r="I16" s="36">
         <f>H16*(G16/100)</f>
         <v>176865.43500000003</v>
       </c>
-      <c r="J16" s="31">
+      <c r="J16" s="38">
         <f>H16-I16</f>
         <v>7392269.5650000023</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="39"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="9" t="s">
         <v>31</v>
       </c>
@@ -2618,8 +2642,8 @@
       </c>
       <c r="G17" s="30"/>
       <c r="H17" s="30"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="40"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="42"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H18">
@@ -2628,17 +2652,17 @@
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="35"/>
-      <c r="J19" s="35"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
     </row>
     <row r="20" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B20" s="27" t="s">
@@ -2647,9 +2671,9 @@
       <c r="C20" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
       <c r="G20" s="27" t="s">
         <v>36</v>
       </c>
@@ -2670,9 +2694,9 @@
       <c r="C21" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="35"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
       <c r="G21">
         <f>(I21/H21)*100</f>
         <v>5.266393401082115</v>
@@ -2695,9 +2719,9 @@
       <c r="C22" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
-      <c r="F22" s="35"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
       <c r="G22">
         <f>(I22/H22)*100</f>
         <v>3.0184759010224669</v>
@@ -2721,6 +2745,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="J4:J6"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="B19:J19"/>
+    <mergeCell ref="D21:F22"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="J13:J15"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="B16:B17"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="G13:G15"/>
@@ -2737,15 +2770,6 @@
     <mergeCell ref="I4:I6"/>
     <mergeCell ref="I16:I17"/>
     <mergeCell ref="B13:B15"/>
-    <mergeCell ref="J4:J6"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="B19:J19"/>
-    <mergeCell ref="D21:F22"/>
-    <mergeCell ref="D20:F20"/>
-    <mergeCell ref="J13:J15"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="B16:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>